<commit_message>
2016/1/14: added 10 papers on kinect
</commit_message>
<xml_diff>
--- a/Catalogue.xlsx
+++ b/Catalogue.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
   <si>
     <t>Category</t>
   </si>
@@ -62,6 +62,111 @@
   <si>
     <t>AAAI</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assessing the Suitability of the Microsoft Kinect for Calculating Person Specific Body Segment Parameters</t>
+  </si>
+  <si>
+    <t>Sean Clarkson, Jon Wheat, Ben Heller, Simon Choppin</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>ECCV</t>
+  </si>
+  <si>
+    <t>A framework for gait-based recognition using Kinect</t>
+  </si>
+  <si>
+    <t>Dimitris Kastaniotis, Ilias Theodorakopoulosa, Christos Theoharatosb, George Economoua, Spiros Fotopoulos</t>
+  </si>
+  <si>
+    <t>2015.6.2</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>PRL</t>
+  </si>
+  <si>
+    <t>Real Time Gait Recognition System based on Kinect Skeleton Feature</t>
+  </si>
+  <si>
+    <t>Shuming Jiang, Yufei Wang, Yuanyuan Zhang, and Jiande Sun</t>
+  </si>
+  <si>
+    <t>ACCV</t>
+  </si>
+  <si>
+    <t>Detection of gait cycles in treadmill walking using a Kinect</t>
+  </si>
+  <si>
+    <t>Edouard Auvinet, Franck Multon, Carl-Eric Aubin, Jean Meunier, Maxime Raison</t>
+  </si>
+  <si>
+    <t>2014.8.11</t>
+  </si>
+  <si>
+    <t>Gait &amp; posture</t>
+  </si>
+  <si>
+    <t>Person Identification in Natural Static Postures Using Kinect</t>
+  </si>
+  <si>
+    <t>Reddy V R, Chakravarty K, Aniruddha S</t>
+  </si>
+  <si>
+    <t>Fall detection in homes of older adults using the microsoft kinect</t>
+  </si>
+  <si>
+    <t>Erik E. Stone, and Marjorie Skubic</t>
+  </si>
+  <si>
+    <t>Biomedical and Health Informatics, IEEE Journal of</t>
+  </si>
+  <si>
+    <t>Full body gait analysis with Kinect</t>
+  </si>
+  <si>
+    <t>Gabel M, Gilad-Bachrach R, Renshaw E</t>
+  </si>
+  <si>
+    <t>EMBC</t>
+  </si>
+  <si>
+    <t>Instrumenting gait assessment using the Kinect in people living with stroke: reliability and association with balance tests</t>
+  </si>
+  <si>
+    <t>Clark R A, Vernon S, Mentiplay B F</t>
+  </si>
+  <si>
+    <t>Journal of neuroengineering and rehabilitation</t>
+  </si>
+  <si>
+    <t>Person Identification Using Full-Body Motion and Anthropometric Biometrics from Kinect Videos</t>
+  </si>
+  <si>
+    <t>Munsell B C, Temlyakov A, Qu C</t>
+  </si>
+  <si>
+    <t>Reachable workspace in facioscapulohumeral muscular dystrophy (FSHD) by kinect</t>
+  </si>
+  <si>
+    <t>Han J J, Kurillo G, Abresch R T</t>
+  </si>
+  <si>
+    <t>Muscle &amp; nerve</t>
+  </si>
+  <si>
+    <t>Towards skeleton biometric identification using the microsoft kinect sensor</t>
+  </si>
+  <si>
+    <t>Araujo R M, Graña G, Andersson V</t>
+  </si>
+  <si>
+    <t>ACM Symposium on Applied Computing</t>
   </si>
 </sst>
 </file>
@@ -413,18 +518,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="78.125" customWidth="1"/>
-    <col min="5" max="5" width="45.875" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="57.625" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
@@ -480,6 +585,274 @@
       </c>
       <c r="I2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>2014</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5">
+        <v>2014</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7">
+        <v>2014</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8">
+        <v>2015</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9">
+        <v>2012</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10">
+        <v>2015</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>2012</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12">
+        <v>2015</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13">
+        <v>2013</v>
+      </c>
+      <c r="I13" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>